<commit_message>
clean up calendar to plot
</commit_message>
<xml_diff>
--- a/Data/CropCalendar.xlsx
+++ b/Data/CropCalendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/Documents/2019_Garden/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timessam/Documents/USAID/Github/Gardening/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F283BCE-ABC7-BF4E-B8D6-E61BAA8D2F34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D958E4-90A2-2C41-B355-B812B8ADA6C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="460" windowWidth="22640" windowHeight="16260" activeTab="6" xr2:uid="{FE2D7DD3-B03B-6945-BDB6-3909327340C1}"/>
+    <workbookView xWindow="2920" yWindow="460" windowWidth="25560" windowHeight="18480" activeTab="1" xr2:uid="{FE2D7DD3-B03B-6945-BDB6-3909327340C1}"/>
   </bookViews>
   <sheets>
     <sheet name="cropCalendar" sheetId="1" r:id="rId1"/>
@@ -356,8 +356,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3275,8 +3275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7FAB09-E426-1947-96E3-73BD6624F753}">
   <dimension ref="A1:XEN31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3284,21 +3284,17 @@
     <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="2" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="4.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="4.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="4.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -3312,79 +3308,79 @@
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="6">
         <v>43525</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="6">
         <v>43535</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="6">
         <v>43545</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="6">
         <v>43555</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="6">
         <v>43565</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="6">
         <v>43575</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="6">
         <v>43585</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="6">
         <v>43595</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="6">
         <v>43605</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="6">
         <v>43615</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="6">
         <v>43625</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="6">
         <v>43635</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="6">
         <v>43645</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="6">
         <v>43655</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="6">
         <v>43665</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="6">
         <v>43675</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="6">
         <v>43685</v>
       </c>
-      <c r="U1" s="5">
+      <c r="U1" s="6">
         <v>43695</v>
       </c>
-      <c r="V1" s="5">
+      <c r="V1" s="6">
         <v>43705</v>
       </c>
-      <c r="W1" s="5">
+      <c r="W1" s="6">
         <v>43715</v>
       </c>
-      <c r="X1" s="5">
+      <c r="X1" s="6">
         <v>43725</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Y1" s="6">
         <v>43735</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="Z1" s="6">
         <v>43745</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AA1" s="6">
         <v>43755</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AB1" s="6">
         <v>43765</v>
       </c>
     </row>
@@ -3398,63 +3394,63 @@
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3468,79 +3464,79 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB3" s="6" t="s">
+      <c r="D3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3554,49 +3550,49 @@
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
+      <c r="D4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
     </row>
     <row r="5" spans="1:28 16368:16368" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
@@ -3608,67 +3604,67 @@
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB5" s="6" t="s">
+      <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB5" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3682,61 +3678,61 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB6" s="6"/>
+      <c r="D6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB6" s="5"/>
       <c r="XEN6"/>
     </row>
     <row r="7" spans="1:28 16368:16368" ht="12" x14ac:dyDescent="0.15">
@@ -3749,69 +3745,69 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6" t="s">
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="U7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="V7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="W7" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="X7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB7" s="6"/>
+      <c r="X7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB7" s="5"/>
     </row>
     <row r="8" spans="1:28 16368:16368" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
@@ -3823,67 +3819,67 @@
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB8" s="5"/>
     </row>
     <row r="9" spans="1:28 16368:16368" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
@@ -3895,63 +3891,63 @@
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB9" s="6" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB9" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3965,63 +3961,63 @@
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB10" s="6" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB10" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4035,73 +4031,73 @@
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB11" s="6" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB11" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4115,63 +4111,63 @@
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB12" s="6" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB12" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4185,67 +4181,67 @@
       <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB13" s="6" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB13" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4259,61 +4255,61 @@
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T14" s="6" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="U14" s="6" t="s">
+      <c r="U14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB14" s="6" t="s">
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB14" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4327,59 +4323,59 @@
       <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB15" s="6" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB15" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4393,61 +4389,61 @@
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB16" s="6" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB16" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4461,65 +4457,65 @@
       <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
     </row>
     <row r="18" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
@@ -4531,65 +4527,65 @@
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
     </row>
     <row r="19" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
@@ -4601,67 +4597,67 @@
       <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
     </row>
     <row r="20" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
@@ -4673,67 +4669,67 @@
       <c r="C20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="U20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="V20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB20" s="5"/>
     </row>
     <row r="21" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
@@ -4745,65 +4741,65 @@
       <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
     </row>
     <row r="22" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
@@ -4815,65 +4811,65 @@
       <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
     </row>
     <row r="23" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
@@ -4885,65 +4881,65 @@
       <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
     </row>
     <row r="24" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
@@ -4955,65 +4951,65 @@
       <c r="C24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
     </row>
     <row r="25" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
@@ -5025,65 +5021,65 @@
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB25" s="6"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB25" s="5"/>
     </row>
     <row r="26" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
@@ -5095,65 +5091,65 @@
       <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="U26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="V26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z26" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
     </row>
     <row r="27" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -5165,63 +5161,63 @@
       <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
     </row>
     <row r="28" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
@@ -5233,59 +5229,59 @@
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA28" s="6"/>
-      <c r="AB28" s="6"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z28" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
     </row>
     <row r="29" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
@@ -5297,65 +5293,65 @@
       <c r="C29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P29" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q29" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA29" s="6"/>
-      <c r="AB29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
     </row>
     <row r="30" spans="1:28" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
@@ -5367,86 +5363,86 @@
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="X30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA30" s="6"/>
-      <c r="AB30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
     </row>
     <row r="31" spans="1:28" ht="12" x14ac:dyDescent="0.15">
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6"/>
-      <c r="AA31" s="6"/>
-      <c r="AB31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:AB30">
@@ -5693,7 +5689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904299B-A4C2-5648-95DB-C334CF58EDFA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>